<commit_message>
Effects doc finished. + Cleaned all class skills doc to fix some effects name.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
@@ -555,6 +555,76 @@
     </r>
   </si>
   <si>
+    <t>[[Area of effect: - Square of 1 cell around the summon ]]</t>
+  </si>
+  <si>
+    <t>Boost the AP of the allies and enemies and increase the ''Power Supply'' level effect of Cyborgs.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Stimulated]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Cyborg: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Power Supply]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>If is a Cyborg:</t>
+  </si>
+  <si>
+    <t>Heal Light-type a target.                                                                        Heals given are proportionate to the target maximum health.            The healing is more effective on the caster or an adjacent entity.                               The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self: </t>
+  </si>
+  <si>
+    <t>If targeting caster or adjacent entity:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Heal: 10% HP]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Else: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Heal: 5% HP]]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">    </t>
     </r>
@@ -565,7 +635,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Binding]]</t>
+      <t>[[Power Supply]]</t>
     </r>
     <r>
       <rPr>
@@ -574,16 +644,65 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve"> -6 levels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Checkpoint]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">          Save the position of the target and teleport it to that position at the end of his turn.                                                                                      Inflicts Light-type damage to the target at the end of his turn if he didn't successfully teleport at the checkpoint position.                                                                                The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>''Force Field Glyph'' (Active Glyph) (1 turn)</t>
+  </si>
+  <si>
+    <t>''Checkpoint Glyph'' (Passive Glyph) (1 turn)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Heavy]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve"> (00 turns)</t>
     </r>
   </si>
   <si>
-    <t>[[Area of effect: - Square of 1 cell around the summon ]]</t>
-  </si>
-  <si>
-    <t>Boost the AP of the allies and enemies and increase the ''Power Supply'' level effect of Cyborgs.</t>
-  </si>
-  <si>
+    <r>
+      <t xml:space="preserve">Active glyph: </t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -591,7 +710,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Stimulated]]</t>
+      <t>[[Heavy]]</t>
     </r>
     <r>
       <rPr>
@@ -600,127 +719,8 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +2 levels (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    Cyborg: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Power Supply]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +2 levels (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <t>If is a Cyborg:</t>
-  </si>
-  <si>
-    <t>Heal Light-type a target.                                                                        Heals given are proportionate to the target maximum health.            The healing is more effective on the caster or an adjacent entity.                               The caster must have enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self: </t>
-  </si>
-  <si>
-    <t>If targeting caster or adjacent entity:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Heal: 10% HP]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Else: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Heal: 5% HP]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Power Supply]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> -6 levels</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Active glyph: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Binding]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve"> (While in the area)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Checkpoint]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">          Save the position of the target and teleport it to that position at the end of his turn.                                                                                      Inflicts Light-type damage to the target at the end of his turn if he didn't successfully teleport at the checkpoint position.                                                                                The caster must have enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
-    <t>''Force Field Glyph'' (Active Glyph) (1 turn)</t>
-  </si>
-  <si>
-    <t>''Checkpoint Glyph'' (Passive Glyph) (1 turn)</t>
   </si>
 </sst>
 </file>
@@ -1488,7 +1488,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1569,7 +1569,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1583,14 +1583,14 @@
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2564,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,7 +2620,7 @@
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2714,7 +2714,7 @@
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -2732,7 +2732,7 @@
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2742,7 +2742,7 @@
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -2754,7 +2754,7 @@
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -2804,7 +2804,7 @@
     <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="24" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2876,7 +2876,7 @@
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C20"/>
+      <selection activeCell="G26" sqref="G26:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,7 +2908,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2996,7 +2996,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -3010,28 +3010,28 @@
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -3192,28 +3192,28 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added class glyph in glyphs doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="9-ForceField" sheetId="9" r:id="rId9"/>
     <sheet name="10-Checkpoint" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,9 +140,6 @@
     <t>[[Number of turns between two casts: 5 ]]</t>
   </si>
   <si>
-    <t>Active glyph: [[Damage:  20 fire ]]</t>
-  </si>
-  <si>
     <t>Charging Point</t>
   </si>
   <si>
@@ -483,12 +480,6 @@
     <t>Teleports the caster.                                                                         Inflicts Fire-type damage to entities on the teleportation path.                        Places aggressive glyphs that inflicts Fire-type damage on the teleportation path.                                                                                                                                                                                                             Consume ''Power Supply'' effect level depending of the target range. Can only select range that the caster as enough ''Power Supply'' effect level to be consumed.</t>
   </si>
   <si>
-    <t>[[Area of effect: - Straight line of cells ]]</t>
-  </si>
-  <si>
-    <t>'Jetpack Glyph'' (Active Glyph) (2 turns) (exclude targeted cell)</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Remove all the remaning AP.</t>
   </si>
   <si>
@@ -700,9 +691,15 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Active glyph: </t>
-    </r>
+    <t>'Burning Ground'' (Active Glyph) (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Straight line of cells ]] (exclude targeted cell)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage:  25 fire ]]</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -710,7 +707,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Heavy]]</t>
+      <t xml:space="preserve">    [[Heavy]]</t>
     </r>
     <r>
       <rPr>
@@ -1306,7 +1303,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1387,28 +1384,28 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1456,7 +1453,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1473,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1488,7 +1485,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1507,7 +1504,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1545,7 +1542,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1569,28 +1566,28 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1670,7 +1667,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1744,28 +1741,28 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1845,7 +1842,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1912,28 +1909,28 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2013,7 +2010,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2080,35 +2077,35 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2191,7 +2188,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2279,21 +2276,21 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2341,7 +2338,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2370,7 @@
     <row r="5" spans="2:4" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2449,7 +2446,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2461,63 +2458,63 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="21" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
       <c r="C27" s="12" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -2580,7 +2577,7 @@
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2595,12 +2592,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2615,12 +2612,12 @@
     <row r="5" spans="2:8" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2647,12 +2644,12 @@
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -2714,7 +2711,7 @@
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -2732,7 +2729,7 @@
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2742,7 +2739,7 @@
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -2754,7 +2751,7 @@
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -2769,49 +2766,49 @@
     <row r="20" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:8" ht="78" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -2896,7 +2893,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2908,7 +2905,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2927,7 +2924,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2996,42 +2993,42 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -3079,7 +3076,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,7 +3096,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -3111,7 +3108,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -3168,7 +3165,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -3180,7 +3177,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -3192,21 +3189,21 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D20" s="1"/>
     </row>

</xml_diff>

<commit_message>
- Finished simplifying the class skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\_Done\10-Cyborg\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sébastien Godbout\Desktop\_MyDev\BattleForVoxturia\GameDesign\Class\_Done\10-Cyborg\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
-  <si>
-    <t>[[AP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Stright line of 1 cell]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
   <si>
     <t>Additional Info</t>
   </si>
@@ -62,9 +56,6 @@
     <t>[[Cast in straight line: No ]]</t>
   </si>
   <si>
-    <t>[[Number of cast per turn per target: 5 ]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Single cell ]]</t>
   </si>
   <si>
@@ -128,12 +119,6 @@
     <t>Jetpack</t>
   </si>
   <si>
-    <t>[[MP: 2 ]]</t>
-  </si>
-  <si>
-    <t>[[AP: 6 ]]</t>
-  </si>
-  <si>
     <t>[[Range: 1-6 ]]</t>
   </si>
   <si>
@@ -173,9 +158,6 @@
     <t>[[Area of effect: - Circle whit 2 cells radius ]]</t>
   </si>
   <si>
-    <t>Entities can't enter or exit the ''Force Field'' area by themself.                                 The ''Force Field'' area move whit the entity having the effect.                           The entities on the ''Force Field'' area can't use self moving abilities except for the entity having the ''Force Field'' effect.                                                                                                     The caster must have enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
     <t>Checkpoint</t>
   </si>
   <si>
@@ -356,6 +338,188 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">    [[Damage: 125 fire ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Caster: Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Power Supply]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>levels to 0</t>
+    </r>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage and attract.</t>
+  </si>
+  <si>
+    <t>Attract by 2 cells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 10-15 ground ]]</t>
+  </si>
+  <si>
+    <t>Enemy:</t>
+  </si>
+  <si>
+    <t>Self:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Teleport to the targeted empty cell.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Power Supply]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -3 levels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">''Charging Point'': </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>[[Area of effect: - Square of 1 cell around the summon ]]</t>
+  </si>
+  <si>
+    <t>Boost the AP of the allies and enemies and increase the ''Power Supply'' level effect of Cyborgs.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Stimulated]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>If is a Cyborg:</t>
+  </si>
+  <si>
+    <t>Heal Light-type a target.                                                                        Heals given are proportionate to the target maximum health.            The healing is more effective on the caster or an adjacent entity.                               The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Heal: 10% HP]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Else: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Heal: 5% HP]]</t>
+  </si>
+  <si>
+    <t>''Force Field Glyph'' (Active Glyph) (1 turn)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Heavy]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>'Burning Ground'' (Active Glyph) (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Straight line of cells ]] (exclude targeted cell)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage:  25 fire ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Heavy]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (While in the area)</t>
+    </r>
+  </si>
+  <si>
+    <t>[[Number of cast per turn: 5 ]]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">If </t>
     </r>
@@ -366,7 +530,15 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Power Supply]] levels</t>
+      <t xml:space="preserve">[[Power Supply]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>levels</t>
     </r>
     <r>
       <rPr>
@@ -379,11 +551,8 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">    [[Damage: 125 fire ]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Caster: Set </t>
+    <r>
+      <t xml:space="preserve">    </t>
     </r>
     <r>
       <rPr>
@@ -392,34 +561,52 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">[[Power Supply]] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>levels to 0</t>
-    </r>
-  </si>
-  <si>
-    <t>Inflicts Ground-type damage and attract.</t>
-  </si>
-  <si>
-    <t>Attract by 2 cells.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage: 10-15 ground ]]</t>
-  </si>
-  <si>
-    <t>Enemy:</t>
-  </si>
-  <si>
-    <t>Self:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Teleport to the targeted empty cell.</t>
+      <t>[[Power Supply]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> -1 levels per Range unit.</t>
+    </r>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>Teleports the caster.                                                                                                Places active glyphs that inflicts Fire-type damage on the teleportation path.                                                                                                                                                                                                             Consume ''Power Supply'' effect level depending of the target range. Can only select range that the caster as enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Cyborg: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Power Supply]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>[[AP: Remaning AP ]]</t>
+  </si>
+  <si>
+    <t>Summons a ''Charging Point'' [[+10% summoner initial Max HP per AP consummed for the summoning, 3 AP, 0 MP, 30% ground resistence,    -15% fire resistence, -50% water resistence, 30% wind resistence, 80% light resistence, 0% dark resistence]]</t>
   </si>
   <si>
     <r>
@@ -441,7 +628,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> -2 levels per Range unit.</t>
+      <t xml:space="preserve"> +(Ap consummed) levels (00 turns)</t>
     </r>
   </si>
   <si>
@@ -455,7 +642,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Invulnerable (Melee)]]</t>
+      <t>[[Power Supply]]</t>
     </r>
     <r>
       <rPr>
@@ -464,23 +651,40 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">    End current turn.</t>
-  </si>
-  <si>
-    <t>Entities between caster and targeted cell:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage: 25-30 fire ]]</t>
-  </si>
-  <si>
-    <t>Teleports the caster.                                                                         Inflicts Fire-type damage to entities on the teleportation path.                        Places aggressive glyphs that inflicts Fire-type damage on the teleportation path.                                                                                                                                                                                                             Consume ''Power Supply'' effect level depending of the target range. Can only select range that the caster as enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Remove all the remaning AP.</t>
+      <t xml:space="preserve"> -1 levels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    If has not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Power Supply]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, set K/O. </t>
+    </r>
+  </si>
+  <si>
+    <t>self or adjacent entity:</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell]]</t>
+  </si>
+  <si>
+    <t>Entities can't enter or exit the ''Force Field'' area by themself.                                                                                                                                                            The caster must have enough ''Power Supply'' effect level to be consumed.</t>
   </si>
   <si>
     <r>
@@ -502,228 +706,23 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> -3 levels</t>
-    </r>
-  </si>
-  <si>
-    <t>Summons a ''Charging Point'' [[+10% summoner HP per AP consummed for the summoning, 3 AP, 0 MP, 30% ground resistence,    -15% fire resistence, -50% water resistence, 30% wind resistence, 80% light resistence, 0% dark resistence]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">''Charging Point'': </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[[Self-Destruction Countdown]] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>((AP consummed) turns)</t>
-    </r>
-  </si>
-  <si>
-    <t>[[Area of effect: - Square of 1 cell around the summon ]]</t>
-  </si>
-  <si>
-    <t>Boost the AP of the allies and enemies and increase the ''Power Supply'' level effect of Cyborgs.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Stimulated]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +2 levels (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    Cyborg: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Power Supply]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +2 levels (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <t>If is a Cyborg:</t>
-  </si>
-  <si>
-    <t>Heal Light-type a target.                                                                        Heals given are proportionate to the target maximum health.            The healing is more effective on the caster or an adjacent entity.                               The caster must have enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self: </t>
-  </si>
-  <si>
-    <t>If targeting caster or adjacent entity:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Heal: 10% HP]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Else: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Heal: 5% HP]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Power Supply]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> -6 levels</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Checkpoint]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">          Save the position of the target and teleport it to that position at the end of his turn.                                                                                      Inflicts Light-type damage to the target at the end of his turn if he didn't successfully teleport at the checkpoint position.                                                                                The caster must have enough ''Power Supply'' effect level to be consumed.</t>
-  </si>
-  <si>
-    <t>''Force Field Glyph'' (Active Glyph) (1 turn)</t>
-  </si>
-  <si>
-    <t>''Checkpoint Glyph'' (Passive Glyph) (1 turn)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Heavy]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (00 turns)</t>
-    </r>
-  </si>
-  <si>
-    <t>'Burning Ground'' (Active Glyph) (2 turns)</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Straight line of cells ]] (exclude targeted cell)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage:  25 fire ]]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    [[Heavy]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (While in the area)</t>
-    </r>
+      <t xml:space="preserve"> -5 levels</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">          Save the position and teleport there at the end of the turn.                                                                                                                                                                      The caster must have enough ''Power Supply'' effect level to be consumed.</t>
+  </si>
+  <si>
+    <t>''Checkpoint Glyph'' (Passive Glyph) (self turn)</t>
+  </si>
+  <si>
+    <t>Teleport to the targeted cell at the end of the turn.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -897,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -954,6 +953,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1267,14 +1270,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1291,7 +1294,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1303,7 +1306,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1315,14 +1318,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1334,21 +1337,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1360,7 +1363,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1372,7 +1375,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1384,28 +1387,28 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1423,7 +1426,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1449,14 +1452,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1473,7 +1476,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1482,10 +1485,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1497,14 +1500,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1516,21 +1519,19 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1542,87 +1543,75 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
+      <c r="C16" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="23" t="s">
+        <v>69</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="15" t="s">
-        <v>93</v>
+      <c r="C18" s="25" t="s">
+        <v>102</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="23" t="s">
-        <v>83</v>
+      <c r="C19" s="27" t="s">
+        <v>103</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="9" t="s">
-        <v>99</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="C25" s="7"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="5"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1631,14 +1620,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1655,7 +1644,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1667,7 +1656,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1679,14 +1668,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1698,7 +1687,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1710,94 +1699,87 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="11" t="s">
-        <v>57</v>
+      <c r="C17" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="12" t="s">
-        <v>58</v>
+      <c r="C18" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="11" t="s">
-        <v>55</v>
+      <c r="C19" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="15" t="s">
-        <v>56</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1806,14 +1788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1830,7 +1812,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1842,7 +1824,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1854,14 +1836,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1873,7 +1855,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1885,7 +1867,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1897,7 +1879,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1909,28 +1891,28 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1948,7 +1930,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1974,14 +1956,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1998,7 +1980,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2010,7 +1992,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2022,14 +2004,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2041,7 +2023,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2053,7 +2035,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2065,7 +2047,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2077,35 +2059,35 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="13" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="12" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="15" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2123,7 +2105,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2152,14 +2134,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2176,7 +2158,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2188,7 +2170,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2200,14 +2182,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2219,21 +2201,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2245,14 +2227,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2264,7 +2246,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2276,21 +2258,21 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2308,7 +2290,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2334,14 +2316,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="87.5703125" customWidth="1"/>
@@ -2358,7 +2340,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2367,10 +2349,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="136.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2382,21 +2364,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2408,21 +2390,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2434,7 +2416,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2446,7 +2428,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2458,63 +2440,53 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
-        <v>77</v>
+      <c r="C22" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
-        <v>78</v>
+      <c r="C23" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="11" t="s">
-        <v>79</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="1"/>
-      <c r="C25" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="21" t="s">
-        <v>104</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="12" t="s">
-        <v>106</v>
+      <c r="C27" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -2523,33 +2495,15 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B29" s="1"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="1"/>
+    </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B31" s="1"/>
-      <c r="C31" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B33" s="1"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="5"/>
+      <c r="D30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2558,14 +2512,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="87.5703125" customWidth="1"/>
@@ -2577,7 +2531,7 @@
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2592,12 +2546,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2612,12 +2566,12 @@
     <row r="5" spans="2:8" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="8" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2632,24 +2586,24 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -2664,19 +2618,19 @@
     <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
@@ -2686,12 +2640,12 @@
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -2706,12 +2660,12 @@
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -2729,7 +2683,7 @@
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="17" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -2739,105 +2693,108 @@
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="18" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="26" t="s">
+        <v>76</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="22" t="s">
-        <v>74</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="22" t="s">
-        <v>82</v>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F21" s="1"/>
+      <c r="G21" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="23" t="s">
-        <v>83</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" ht="78" x14ac:dyDescent="0.4">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="14" t="s">
-        <v>84</v>
+      <c r="C23" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="24" t="s">
-        <v>85</v>
+      <c r="C24" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:8" ht="78" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="24" t="s">
-        <v>103</v>
+      <c r="C25" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="22" t="s">
-        <v>86</v>
+      <c r="C26" s="24" t="s">
+        <v>70</v>
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B28" s="1"/>
+      <c r="C28" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B30" s="1"/>
-      <c r="C30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="1"/>
-    </row>
+    </row>
+    <row r="30" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2846,21 +2803,41 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B32" s="1"/>
-      <c r="C32" s="7"/>
+      <c r="C32" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="7"/>
+      <c r="G32" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="5"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B34" s="1"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="5"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2869,14 +2846,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G28"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2893,7 +2870,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2905,7 +2882,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2917,14 +2894,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2936,21 +2913,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2962,14 +2939,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2981,7 +2958,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2993,42 +2970,42 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="23" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="15" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="15" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="15" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="15" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -3046,7 +3023,7 @@
     <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
       <c r="C28" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -3072,14 +3049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -3096,7 +3073,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -3105,10 +3082,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -3120,14 +3097,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -3139,21 +3116,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -3165,7 +3142,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -3177,7 +3154,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -3189,28 +3166,28 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="15" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="21" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="12" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -3228,7 +3205,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>

</xml_diff>

<commit_message>
- Defined 2 roles for each class. - Finished the Roles section in the NewCharacterCreation screen.
- Next task is to define the class description and fix all the game text for TMP...
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
+++ b/GameDesign/Class/_Done/10-Cyborg/Documentation/CyborgSkills.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Recharge " sheetId="1" r:id="rId1"/>
@@ -1273,7 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1455,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2849,7 +2849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>